<commit_message>
fixed glucose unit issues
</commit_message>
<xml_diff>
--- a/data/raw/Project_S.xlsx
+++ b/data/raw/Project_S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R&amp;D Services\06_KEYSTONE&amp;CLD\OU project\SEQ_30 Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DE9BEB-60A4-4ADC-8FE5-E07352AFCBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF5BA17-4B67-4E0A-B143-D8069CB9A2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{41BC70CE-2FB0-4EDB-AD74-6F3C710D7155}"/>
   </bookViews>
@@ -16042,8 +16042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C5B42F-905F-4F32-B5AA-B8120AA1EAE6}">
   <dimension ref="A1:AP153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M34" workbookViewId="0">
-      <selection activeCell="R129" sqref="R129"/>
+    <sheetView tabSelected="1" topLeftCell="S120" workbookViewId="0">
+      <selection activeCell="AH143" sqref="AH143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16962,7 +16962,7 @@
         <v>13.2</v>
       </c>
       <c r="AI10" s="7">
-        <v>22.4</v>
+        <v>2.24E-2</v>
       </c>
       <c r="AJ10" s="71"/>
       <c r="AK10" s="71"/>
@@ -17064,7 +17064,7 @@
         <v>10.5</v>
       </c>
       <c r="AI11" s="7">
-        <v>10881</v>
+        <v>10.88</v>
       </c>
       <c r="AJ11" s="71"/>
       <c r="AK11" s="71"/>
@@ -17166,7 +17166,7 @@
         <v>5.5</v>
       </c>
       <c r="AI12" s="7">
-        <v>1550</v>
+        <v>1.55</v>
       </c>
       <c r="AJ12" s="71"/>
       <c r="AK12" s="71"/>
@@ -17666,7 +17666,7 @@
         <v>0</v>
       </c>
       <c r="AI17" s="7">
-        <v>21149</v>
+        <v>21.149000000000001</v>
       </c>
       <c r="AJ17" s="71"/>
       <c r="AK17" s="71"/>
@@ -17864,7 +17864,7 @@
         <v>0</v>
       </c>
       <c r="AI19" s="7">
-        <v>21354</v>
+        <v>21.353999999999999</v>
       </c>
       <c r="AJ19" s="71"/>
       <c r="AK19" s="71"/>
@@ -18060,7 +18060,7 @@
       <c r="AG21" s="7"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="7">
-        <v>6.4</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AJ21" s="71"/>
       <c r="AK21" s="71"/>
@@ -18256,7 +18256,7 @@
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
       <c r="AI23" s="7">
-        <v>13.4</v>
+        <v>0.1</v>
       </c>
       <c r="AJ23" s="71"/>
       <c r="AK23" s="71"/>
@@ -18452,7 +18452,7 @@
       <c r="AG25" s="7"/>
       <c r="AH25" s="7"/>
       <c r="AI25" s="7">
-        <v>12.2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AJ25" s="71"/>
       <c r="AK25" s="71"/>
@@ -18648,7 +18648,7 @@
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
       <c r="AI27" s="7">
-        <v>12.8</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AJ27" s="71"/>
       <c r="AK27" s="71"/>
@@ -18757,7 +18757,7 @@
       <c r="AG28" s="7"/>
       <c r="AH28" s="7"/>
       <c r="AI28" s="7">
-        <v>9.6</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AJ28" s="71"/>
       <c r="AK28" s="71"/>
@@ -19551,7 +19551,7 @@
         <v>11.4</v>
       </c>
       <c r="AI36" s="42">
-        <v>4558</v>
+        <v>4.55</v>
       </c>
       <c r="AJ36" s="75"/>
       <c r="AK36" s="71"/>
@@ -19653,7 +19653,7 @@
         <v>8.5</v>
       </c>
       <c r="AI37" s="42">
-        <v>802</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="AJ37" s="75"/>
       <c r="AK37" s="71"/>
@@ -20153,7 +20153,7 @@
         <v>4.2</v>
       </c>
       <c r="AI42" s="42">
-        <v>14231</v>
+        <v>14.23</v>
       </c>
       <c r="AJ42" s="71"/>
       <c r="AK42" s="71"/>
@@ -20349,7 +20349,7 @@
       <c r="AG44" s="42"/>
       <c r="AH44" s="42"/>
       <c r="AI44" s="42">
-        <v>8503</v>
+        <v>8.5</v>
       </c>
       <c r="AJ44" s="71"/>
       <c r="AK44" s="71"/>
@@ -20545,7 +20545,7 @@
       <c r="AG46" s="42"/>
       <c r="AH46" s="42"/>
       <c r="AI46" s="42">
-        <v>12.8</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AJ46" s="71"/>
       <c r="AK46" s="71"/>
@@ -20741,7 +20741,7 @@
       <c r="AG48" s="42"/>
       <c r="AH48" s="42"/>
       <c r="AI48" s="42">
-        <v>11.5</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AJ48" s="71"/>
       <c r="AK48" s="71"/>
@@ -20937,7 +20937,7 @@
       <c r="AG50" s="42"/>
       <c r="AH50" s="42"/>
       <c r="AI50" s="42">
-        <v>12.8</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="AJ50" s="71"/>
       <c r="AK50" s="71"/>
@@ -21133,7 +21133,7 @@
       <c r="AG52" s="42"/>
       <c r="AH52" s="42"/>
       <c r="AI52" s="42">
-        <v>9.6</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AJ52" s="71"/>
       <c r="AK52" s="71"/>
@@ -21241,7 +21241,7 @@
       <c r="AG53" s="42"/>
       <c r="AH53" s="42"/>
       <c r="AI53" s="42">
-        <v>7.7</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AJ53" s="71"/>
       <c r="AK53" s="71"/>
@@ -22035,7 +22035,7 @@
         <v>11.9</v>
       </c>
       <c r="AI61" s="18">
-        <v>1036</v>
+        <v>1</v>
       </c>
       <c r="AJ61" s="71"/>
       <c r="AK61" s="71"/>
@@ -22137,7 +22137,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="AI62" s="18">
-        <v>670</v>
+        <v>0.6</v>
       </c>
       <c r="AJ62" s="71"/>
       <c r="AK62" s="71"/>
@@ -22637,7 +22637,7 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="AI67" s="18">
-        <v>14231</v>
+        <v>14.23</v>
       </c>
       <c r="AJ67" s="71"/>
       <c r="AK67" s="71"/>
@@ -22833,7 +22833,7 @@
       <c r="AG69" s="18"/>
       <c r="AH69" s="17"/>
       <c r="AI69" s="18">
-        <v>8516</v>
+        <v>8.516</v>
       </c>
       <c r="AJ69" s="71"/>
       <c r="AK69" s="71"/>
@@ -23029,7 +23029,7 @@
       <c r="AG71" s="18"/>
       <c r="AH71" s="17"/>
       <c r="AI71" s="18">
-        <v>13</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="AJ71" s="71"/>
       <c r="AK71" s="71"/>
@@ -23225,7 +23225,7 @@
       <c r="AG73" s="18"/>
       <c r="AH73" s="17"/>
       <c r="AI73" s="18">
-        <v>12</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="AJ73" s="71"/>
       <c r="AK73" s="71"/>
@@ -23421,7 +23421,7 @@
       <c r="AG75" s="18"/>
       <c r="AH75" s="17"/>
       <c r="AI75" s="18">
-        <v>11</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AJ75" s="71"/>
       <c r="AK75" s="71"/>
@@ -23617,7 +23617,7 @@
       <c r="AG77" s="18"/>
       <c r="AH77" s="18"/>
       <c r="AI77" s="18">
-        <v>13</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="AJ77" s="71"/>
       <c r="AK77" s="71"/>
@@ -23725,7 +23725,7 @@
       <c r="AG78" s="18"/>
       <c r="AH78" s="18"/>
       <c r="AI78" s="18">
-        <v>10</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ78" s="71"/>
       <c r="AK78" s="71"/>
@@ -24213,7 +24213,7 @@
         <v>18.3</v>
       </c>
       <c r="AI83" s="49">
-        <v>6071</v>
+        <v>0.6</v>
       </c>
       <c r="AJ83" s="71"/>
       <c r="AK83" s="71"/>
@@ -24417,7 +24417,7 @@
         <v>9.5</v>
       </c>
       <c r="AI85" s="49">
-        <v>2275</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AJ85" s="71"/>
       <c r="AK85" s="71"/>
@@ -24519,7 +24519,7 @@
         <v>7.3</v>
       </c>
       <c r="AI86" s="49">
-        <v>3168</v>
+        <v>3.1</v>
       </c>
       <c r="AJ86" s="71"/>
       <c r="AK86" s="71"/>
@@ -24825,7 +24825,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="AI89" s="49">
-        <v>2500</v>
+        <v>2.5</v>
       </c>
       <c r="AJ89" s="71"/>
       <c r="AK89" s="71"/>
@@ -24929,7 +24929,7 @@
         <v>6.2</v>
       </c>
       <c r="AI90" s="49">
-        <v>8874</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="AJ90" s="71"/>
       <c r="AK90" s="71"/>
@@ -25127,7 +25127,7 @@
         <v>4.2</v>
       </c>
       <c r="AI92" s="49">
-        <v>14231</v>
+        <v>14.23</v>
       </c>
       <c r="AJ92" s="71"/>
       <c r="AK92" s="71"/>
@@ -25519,7 +25519,7 @@
       <c r="AG96" s="49"/>
       <c r="AH96" s="49"/>
       <c r="AI96" s="49">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AJ96" s="71"/>
       <c r="AK96" s="71"/>
@@ -25715,7 +25715,7 @@
       <c r="AG98" s="49"/>
       <c r="AH98" s="49"/>
       <c r="AI98" s="49">
-        <v>14</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ98" s="71"/>
       <c r="AK98" s="71"/>
@@ -25911,7 +25911,7 @@
       <c r="AG100" s="49"/>
       <c r="AH100" s="49"/>
       <c r="AI100" s="49">
-        <v>15</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ100" s="71"/>
       <c r="AK100" s="71"/>
@@ -26107,7 +26107,7 @@
       <c r="AG102" s="49"/>
       <c r="AH102" s="49"/>
       <c r="AI102" s="49">
-        <v>15</v>
+        <v>1.5E-3</v>
       </c>
       <c r="AJ102" s="71"/>
       <c r="AK102" s="71"/>
@@ -26216,7 +26216,7 @@
       <c r="AG103" s="49"/>
       <c r="AH103" s="49"/>
       <c r="AI103" s="52">
-        <v>17</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="AJ103" s="71"/>
       <c r="AK103" s="71"/>
@@ -26709,7 +26709,7 @@
         <v>20.8</v>
       </c>
       <c r="AI108" s="54">
-        <v>9858</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AJ108" s="71"/>
       <c r="AK108" s="71"/>
@@ -26812,7 +26812,7 @@
         <v>20.5</v>
       </c>
       <c r="AI109" s="54">
-        <v>21999</v>
+        <v>21.99</v>
       </c>
       <c r="AJ109" s="71"/>
       <c r="AK109" s="71"/>
@@ -26915,7 +26915,7 @@
         <v>24</v>
       </c>
       <c r="AI110" s="54">
-        <v>24582</v>
+        <v>24.52</v>
       </c>
       <c r="AJ110" s="71"/>
       <c r="AK110" s="71"/>
@@ -27018,7 +27018,7 @@
         <v>25.5</v>
       </c>
       <c r="AI111" s="54">
-        <v>24186</v>
+        <v>24.18</v>
       </c>
       <c r="AJ111" s="71"/>
       <c r="AK111" s="71"/>
@@ -27121,7 +27121,7 @@
         <v>26.3</v>
       </c>
       <c r="AI112" s="54">
-        <v>24115</v>
+        <v>24.11</v>
       </c>
       <c r="AJ112" s="71"/>
       <c r="AK112" s="71"/>
@@ -27224,7 +27224,7 @@
         <v>26.6</v>
       </c>
       <c r="AI113" s="54">
-        <v>24147</v>
+        <v>24.14</v>
       </c>
       <c r="AJ113" s="71"/>
       <c r="AK113" s="71"/>
@@ -27798,7 +27798,7 @@
       <c r="AG119" s="54"/>
       <c r="AH119" s="54"/>
       <c r="AI119" s="54">
-        <v>23636</v>
+        <v>23.36</v>
       </c>
       <c r="AJ119" s="71"/>
       <c r="AK119" s="71"/>
@@ -28672,7 +28672,7 @@
       <c r="AG128" s="54"/>
       <c r="AH128" s="54"/>
       <c r="AI128" s="54">
-        <v>96</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AJ128" s="71"/>
       <c r="AK128" s="71"/>
@@ -29165,7 +29165,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="AI133" s="57">
-        <v>5818</v>
+        <v>5.8</v>
       </c>
       <c r="AJ133" s="71"/>
       <c r="AK133" s="71"/>
@@ -29268,7 +29268,7 @@
         <v>12.2</v>
       </c>
       <c r="AI134" s="57">
-        <v>675</v>
+        <v>0.67</v>
       </c>
       <c r="AJ134" s="71"/>
       <c r="AK134" s="71"/>
@@ -29371,7 +29371,7 @@
         <v>13.3</v>
       </c>
       <c r="AI135" s="57">
-        <v>1908</v>
+        <v>1.9</v>
       </c>
       <c r="AJ135" s="71"/>
       <c r="AK135" s="71"/>
@@ -29474,7 +29474,7 @@
         <v>9.6</v>
       </c>
       <c r="AI136" s="57">
-        <v>4039</v>
+        <v>4</v>
       </c>
       <c r="AJ136" s="71"/>
       <c r="AK136" s="71"/>
@@ -30088,7 +30088,7 @@
         <v>0</v>
       </c>
       <c r="AI142" s="57">
-        <v>1460</v>
+        <v>1.4</v>
       </c>
       <c r="AJ142" s="71"/>
       <c r="AK142" s="71"/>
@@ -30286,7 +30286,7 @@
       <c r="AG144" s="57"/>
       <c r="AH144" s="57"/>
       <c r="AI144" s="57">
-        <v>70</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AJ144" s="71"/>
       <c r="AK144" s="71"/>
@@ -30484,7 +30484,7 @@
       <c r="AG146" s="57"/>
       <c r="AH146" s="57"/>
       <c r="AI146" s="57">
-        <v>10</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ146" s="71"/>
       <c r="AK146" s="71"/>
@@ -30682,7 +30682,7 @@
       <c r="AG148" s="57"/>
       <c r="AH148" s="57"/>
       <c r="AI148" s="57">
-        <v>11</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ148" s="71"/>
       <c r="AK148" s="71"/>
@@ -30880,7 +30880,7 @@
       <c r="AG150" s="57"/>
       <c r="AH150" s="57"/>
       <c r="AI150" s="57">
-        <v>12</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ150" s="71"/>
       <c r="AK150" s="71"/>
@@ -31078,7 +31078,7 @@
       <c r="AG152" s="57"/>
       <c r="AH152" s="57"/>
       <c r="AI152" s="57">
-        <v>15</v>
+        <v>1.5E-3</v>
       </c>
       <c r="AJ152" s="71"/>
       <c r="AK152" s="71"/>
@@ -31188,7 +31188,7 @@
       <c r="AG153" s="57"/>
       <c r="AH153" s="57"/>
       <c r="AI153" s="57">
-        <v>12</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="AJ153" s="71"/>
       <c r="AK153" s="71"/>

</xml_diff>